<commit_message>
new store numbers formatted
</commit_message>
<xml_diff>
--- a/data/misc/Store Numbers/Clean/IAE/zaxbys.xlsx
+++ b/data/misc/Store Numbers/Clean/IAE/zaxbys.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="435" windowWidth="19875" windowHeight="8925"/>
@@ -2497,15 +2497,6 @@
     <t>JEFFERSON CITY</t>
   </si>
   <si>
-    <t>Keyword</t>
-  </si>
-  <si>
-    <t>Agg store_number</t>
-  </si>
-  <si>
-    <t>Store number</t>
-  </si>
-  <si>
     <t>#0019901 19901 #019901 #19901 0019901</t>
   </si>
   <si>
@@ -3794,6 +3785,15 @@
   </si>
   <si>
     <t>#0038901 38901 #038901 #38901 0038901</t>
+  </si>
+  <si>
+    <t>keywords</t>
+  </si>
+  <si>
+    <t>Aggdata Store Number</t>
+  </si>
+  <si>
+    <t>store_number</t>
   </si>
 </sst>
 </file>
@@ -4625,26 +4625,32 @@
   <dimension ref="A1:G491"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>826</v>
+        <v>1256</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>827</v>
+        <v>1257</v>
       </c>
       <c r="D1" t="s">
-        <v>828</v>
+        <v>1258</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -4667,7 +4673,7 @@
         <v>19901</v>
       </c>
       <c r="D2" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="E2" t="s">
         <v>727</v>
@@ -4690,7 +4696,7 @@
         <v>34701</v>
       </c>
       <c r="D3" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="E3" t="s">
         <v>516</v>
@@ -4713,7 +4719,7 @@
         <v>303</v>
       </c>
       <c r="D4" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="E4" t="s">
         <v>117</v>
@@ -4736,7 +4742,7 @@
         <v>305</v>
       </c>
       <c r="D5" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="E5" t="s">
         <v>119</v>
@@ -4759,7 +4765,7 @@
         <v>306</v>
       </c>
       <c r="D6" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="E6" t="s">
         <v>121</v>
@@ -4782,7 +4788,7 @@
         <v>503</v>
       </c>
       <c r="D7" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="E7" t="s">
         <v>676</v>
@@ -4805,7 +4811,7 @@
         <v>504</v>
       </c>
       <c r="D8" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="E8" t="s">
         <v>124</v>
@@ -4828,7 +4834,7 @@
         <v>1201</v>
       </c>
       <c r="D9" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="E9" t="s">
         <v>134</v>
@@ -4851,7 +4857,7 @@
         <v>1301</v>
       </c>
       <c r="D10" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="E10" t="s">
         <v>136</v>
@@ -4874,7 +4880,7 @@
         <v>1305</v>
       </c>
       <c r="D11" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="E11" t="s">
         <v>140</v>
@@ -4897,7 +4903,7 @@
         <v>1306</v>
       </c>
       <c r="D12" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="E12" t="s">
         <v>141</v>
@@ -4920,7 +4926,7 @@
         <v>1308</v>
       </c>
       <c r="D13" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="E13" t="s">
         <v>144</v>
@@ -4943,7 +4949,7 @@
         <v>10101</v>
       </c>
       <c r="D14" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="E14" t="s">
         <v>246</v>
@@ -4966,7 +4972,7 @@
         <v>10201</v>
       </c>
       <c r="D15" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="E15" t="s">
         <v>248</v>
@@ -4989,7 +4995,7 @@
         <v>10501</v>
       </c>
       <c r="D16" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="E16" t="s">
         <v>251</v>
@@ -5012,7 +5018,7 @@
         <v>20101</v>
       </c>
       <c r="D17" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="E17" t="s">
         <v>729</v>
@@ -5035,7 +5041,7 @@
         <v>21401</v>
       </c>
       <c r="D18" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="E18" t="s">
         <v>734</v>
@@ -5058,7 +5064,7 @@
         <v>801</v>
       </c>
       <c r="D19" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="E19" t="s">
         <v>130</v>
@@ -5081,7 +5087,7 @@
         <v>102</v>
       </c>
       <c r="D20" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
@@ -5104,7 +5110,7 @@
         <v>103</v>
       </c>
       <c r="D21" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -5127,7 +5133,7 @@
         <v>104</v>
       </c>
       <c r="D22" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="E22" t="s">
         <v>637</v>
@@ -5150,7 +5156,7 @@
         <v>105</v>
       </c>
       <c r="D23" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -5173,7 +5179,7 @@
         <v>106</v>
       </c>
       <c r="D24" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
@@ -5196,7 +5202,7 @@
         <v>107</v>
       </c>
       <c r="D25" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="E25" t="s">
         <v>14</v>
@@ -5219,7 +5225,7 @@
         <v>108</v>
       </c>
       <c r="D26" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="E26" t="s">
         <v>15</v>
@@ -5242,7 +5248,7 @@
         <v>109</v>
       </c>
       <c r="D27" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="E27" t="s">
         <v>17</v>
@@ -5265,7 +5271,7 @@
         <v>110</v>
       </c>
       <c r="D28" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="E28" t="s">
         <v>639</v>
@@ -5288,7 +5294,7 @@
         <v>111</v>
       </c>
       <c r="D29" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="E29" t="s">
         <v>20</v>
@@ -5311,7 +5317,7 @@
         <v>113</v>
       </c>
       <c r="D30" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="E30" t="s">
         <v>22</v>
@@ -5334,7 +5340,7 @@
         <v>115</v>
       </c>
       <c r="D31" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="E31" t="s">
         <v>24</v>
@@ -5357,7 +5363,7 @@
         <v>116</v>
       </c>
       <c r="D32" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="E32" t="s">
         <v>25</v>
@@ -5380,7 +5386,7 @@
         <v>117</v>
       </c>
       <c r="D33" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="E33" t="s">
         <v>640</v>
@@ -5403,7 +5409,7 @@
         <v>118</v>
       </c>
       <c r="D34" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="E34" t="s">
         <v>26</v>
@@ -5426,7 +5432,7 @@
         <v>119</v>
       </c>
       <c r="D35" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="E35" t="s">
         <v>642</v>
@@ -5449,7 +5455,7 @@
         <v>120</v>
       </c>
       <c r="D36" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="E36" t="s">
         <v>28</v>
@@ -5472,7 +5478,7 @@
         <v>121</v>
       </c>
       <c r="D37" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="E37" t="s">
         <v>644</v>
@@ -5495,7 +5501,7 @@
         <v>122</v>
       </c>
       <c r="D38" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="E38" t="s">
         <v>30</v>
@@ -5518,7 +5524,7 @@
         <v>123</v>
       </c>
       <c r="D39" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="E39" t="s">
         <v>32</v>
@@ -5541,7 +5547,7 @@
         <v>124</v>
       </c>
       <c r="D40" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="E40" t="s">
         <v>34</v>
@@ -5564,7 +5570,7 @@
         <v>126</v>
       </c>
       <c r="D41" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="E41" t="s">
         <v>646</v>
@@ -5587,7 +5593,7 @@
         <v>127</v>
       </c>
       <c r="D42" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="E42" t="s">
         <v>37</v>
@@ -5610,7 +5616,7 @@
         <v>129</v>
       </c>
       <c r="D43" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="E43" t="s">
         <v>648</v>
@@ -5633,7 +5639,7 @@
         <v>130</v>
       </c>
       <c r="D44" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="E44" t="s">
         <v>39</v>
@@ -5656,7 +5662,7 @@
         <v>131</v>
       </c>
       <c r="D45" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="E45" t="s">
         <v>41</v>
@@ -5679,7 +5685,7 @@
         <v>132</v>
       </c>
       <c r="D46" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="E46" t="s">
         <v>650</v>
@@ -5702,7 +5708,7 @@
         <v>133</v>
       </c>
       <c r="D47" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="E47" t="s">
         <v>652</v>
@@ -5725,7 +5731,7 @@
         <v>134</v>
       </c>
       <c r="D48" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="E48" t="s">
         <v>653</v>
@@ -5748,7 +5754,7 @@
         <v>135</v>
       </c>
       <c r="D49" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="E49" t="s">
         <v>43</v>
@@ -5771,7 +5777,7 @@
         <v>136</v>
       </c>
       <c r="D50" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="E50" t="s">
         <v>655</v>
@@ -5794,7 +5800,7 @@
         <v>137</v>
       </c>
       <c r="D51" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="E51" t="s">
         <v>45</v>
@@ -5817,7 +5823,7 @@
         <v>142</v>
       </c>
       <c r="D52" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="E52" t="s">
         <v>657</v>
@@ -5840,7 +5846,7 @@
         <v>143</v>
       </c>
       <c r="D53" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="E53" t="s">
         <v>658</v>
@@ -5863,7 +5869,7 @@
         <v>145</v>
       </c>
       <c r="D54" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="E54" t="s">
         <v>47</v>
@@ -5886,7 +5892,7 @@
         <v>146</v>
       </c>
       <c r="D55" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="E55" t="s">
         <v>49</v>
@@ -5909,7 +5915,7 @@
         <v>147</v>
       </c>
       <c r="D56" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="E56" t="s">
         <v>51</v>
@@ -5932,7 +5938,7 @@
         <v>148</v>
       </c>
       <c r="D57" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="E57" t="s">
         <v>53</v>
@@ -5955,7 +5961,7 @@
         <v>149</v>
       </c>
       <c r="D58" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="E58" t="s">
         <v>659</v>
@@ -5978,7 +5984,7 @@
         <v>150</v>
       </c>
       <c r="D59" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="E59" t="s">
         <v>661</v>
@@ -6001,7 +6007,7 @@
         <v>151</v>
       </c>
       <c r="D60" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="E60" t="s">
         <v>55</v>
@@ -6024,7 +6030,7 @@
         <v>152</v>
       </c>
       <c r="D61" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="E61" t="s">
         <v>58</v>
@@ -6047,7 +6053,7 @@
         <v>153</v>
       </c>
       <c r="D62" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="E62" t="s">
         <v>59</v>
@@ -6070,7 +6076,7 @@
         <v>154</v>
       </c>
       <c r="D63" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="E63" t="s">
         <v>662</v>
@@ -6093,7 +6099,7 @@
         <v>155</v>
       </c>
       <c r="D64" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="E64" t="s">
         <v>61</v>
@@ -6116,7 +6122,7 @@
         <v>156</v>
       </c>
       <c r="D65" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="E65" t="s">
         <v>664</v>
@@ -6139,7 +6145,7 @@
         <v>157</v>
       </c>
       <c r="D66" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="E66" t="s">
         <v>62</v>
@@ -6162,7 +6168,7 @@
         <v>158</v>
       </c>
       <c r="D67" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="E67" t="s">
         <v>63</v>
@@ -6185,7 +6191,7 @@
         <v>159</v>
       </c>
       <c r="D68" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="E68" t="s">
         <v>666</v>
@@ -6208,7 +6214,7 @@
         <v>160</v>
       </c>
       <c r="D69" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="E69" t="s">
         <v>65</v>
@@ -6231,7 +6237,7 @@
         <v>161</v>
       </c>
       <c r="D70" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="E70" t="s">
         <v>667</v>
@@ -6254,7 +6260,7 @@
         <v>162</v>
       </c>
       <c r="D71" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="E71" t="s">
         <v>67</v>
@@ -6277,7 +6283,7 @@
         <v>163</v>
       </c>
       <c r="D72" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="E72" t="s">
         <v>68</v>
@@ -6300,7 +6306,7 @@
         <v>164</v>
       </c>
       <c r="D73" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="E73" t="s">
         <v>70</v>
@@ -6323,7 +6329,7 @@
         <v>165</v>
       </c>
       <c r="D74" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="E74" t="s">
         <v>669</v>
@@ -6346,7 +6352,7 @@
         <v>166</v>
       </c>
       <c r="D75" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="E75" t="s">
         <v>71</v>
@@ -6369,7 +6375,7 @@
         <v>168</v>
       </c>
       <c r="D76" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="E76" t="s">
         <v>670</v>
@@ -6392,7 +6398,7 @@
         <v>169</v>
       </c>
       <c r="D77" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="E77" t="s">
         <v>73</v>
@@ -6415,7 +6421,7 @@
         <v>171</v>
       </c>
       <c r="D78" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="E78" t="s">
         <v>74</v>
@@ -6438,7 +6444,7 @@
         <v>174</v>
       </c>
       <c r="D79" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="E79" t="s">
         <v>76</v>
@@ -6461,7 +6467,7 @@
         <v>176</v>
       </c>
       <c r="D80" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="E80" t="s">
         <v>78</v>
@@ -6484,7 +6490,7 @@
         <v>177</v>
       </c>
       <c r="D81" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="E81" t="s">
         <v>80</v>
@@ -6507,7 +6513,7 @@
         <v>178</v>
       </c>
       <c r="D82" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="E82" t="s">
         <v>83</v>
@@ -6530,7 +6536,7 @@
         <v>180</v>
       </c>
       <c r="D83" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="E83" t="s">
         <v>85</v>
@@ -6553,7 +6559,7 @@
         <v>181</v>
       </c>
       <c r="D84" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="E84" t="s">
         <v>672</v>
@@ -6576,7 +6582,7 @@
         <v>184</v>
       </c>
       <c r="D85" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="E85" t="s">
         <v>87</v>
@@ -6599,7 +6605,7 @@
         <v>185</v>
       </c>
       <c r="D86" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="E86" t="s">
         <v>674</v>
@@ -6622,7 +6628,7 @@
         <v>186</v>
       </c>
       <c r="D87" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="E87" t="s">
         <v>88</v>
@@ -6645,7 +6651,7 @@
         <v>188</v>
       </c>
       <c r="D88" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="E88" t="s">
         <v>90</v>
@@ -6668,7 +6674,7 @@
         <v>192</v>
       </c>
       <c r="D89" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="E89" t="s">
         <v>92</v>
@@ -6691,7 +6697,7 @@
         <v>193</v>
       </c>
       <c r="D90" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="E90" t="s">
         <v>94</v>
@@ -6714,7 +6720,7 @@
         <v>195</v>
       </c>
       <c r="D91" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="E91" t="s">
         <v>95</v>
@@ -6737,7 +6743,7 @@
         <v>196</v>
       </c>
       <c r="D92" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="E92" t="s">
         <v>98</v>
@@ -6760,7 +6766,7 @@
         <v>197</v>
       </c>
       <c r="D93" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="E93" t="s">
         <v>100</v>
@@ -6783,7 +6789,7 @@
         <v>198</v>
       </c>
       <c r="D94" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="E94" t="s">
         <v>101</v>
@@ -6806,7 +6812,7 @@
         <v>199</v>
       </c>
       <c r="D95" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="E95" t="s">
         <v>103</v>
@@ -6829,7 +6835,7 @@
         <v>201</v>
       </c>
       <c r="D96" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="E96" t="s">
         <v>105</v>
@@ -6852,7 +6858,7 @@
         <v>203</v>
       </c>
       <c r="D97" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="E97" t="s">
         <v>108</v>
@@ -6875,7 +6881,7 @@
         <v>204</v>
       </c>
       <c r="D98" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="E98" t="s">
         <v>109</v>
@@ -6898,7 +6904,7 @@
         <v>205</v>
       </c>
       <c r="D99" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="E99" t="s">
         <v>111</v>
@@ -6921,7 +6927,7 @@
         <v>301</v>
       </c>
       <c r="D100" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="E100" t="s">
         <v>113</v>
@@ -6944,7 +6950,7 @@
         <v>302</v>
       </c>
       <c r="D101" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="E101" t="s">
         <v>115</v>
@@ -6967,7 +6973,7 @@
         <v>304</v>
       </c>
       <c r="D102" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="E102" t="s">
         <v>675</v>
@@ -6990,7 +6996,7 @@
         <v>502</v>
       </c>
       <c r="D103" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="E103" t="s">
         <v>123</v>
@@ -7013,7 +7019,7 @@
         <v>505</v>
       </c>
       <c r="D104" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="E104" t="s">
         <v>125</v>
@@ -7036,7 +7042,7 @@
         <v>601</v>
       </c>
       <c r="D105" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="E105" t="s">
         <v>127</v>
@@ -7059,7 +7065,7 @@
         <v>701</v>
       </c>
       <c r="D106" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="E106" t="s">
         <v>128</v>
@@ -7082,7 +7088,7 @@
         <v>901</v>
       </c>
       <c r="D107" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="E107" t="s">
         <v>132</v>
@@ -7105,7 +7111,7 @@
         <v>1302</v>
       </c>
       <c r="D108" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="E108" t="s">
         <v>138</v>
@@ -7128,7 +7134,7 @@
         <v>1307</v>
       </c>
       <c r="D109" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="E109" t="s">
         <v>143</v>
@@ -7151,7 +7157,7 @@
         <v>1309</v>
       </c>
       <c r="D110" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="E110" t="s">
         <v>146</v>
@@ -7174,7 +7180,7 @@
         <v>1310</v>
       </c>
       <c r="D111" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="E111" t="s">
         <v>147</v>
@@ -7197,7 +7203,7 @@
         <v>1311</v>
       </c>
       <c r="D112" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="E112" t="s">
         <v>678</v>
@@ -7220,7 +7226,7 @@
         <v>1701</v>
       </c>
       <c r="D113" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="E113" t="s">
         <v>149</v>
@@ -7243,7 +7249,7 @@
         <v>1702</v>
       </c>
       <c r="D114" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="E114" t="s">
         <v>679</v>
@@ -7266,7 +7272,7 @@
         <v>1703</v>
       </c>
       <c r="D115" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="E115" t="s">
         <v>150</v>
@@ -7289,7 +7295,7 @@
         <v>1801</v>
       </c>
       <c r="D116" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="E116" t="s">
         <v>680</v>
@@ -7312,7 +7318,7 @@
         <v>1901</v>
       </c>
       <c r="D117" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="E117" t="s">
         <v>151</v>
@@ -7335,7 +7341,7 @@
         <v>2201</v>
       </c>
       <c r="D118" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="E118" t="s">
         <v>682</v>
@@ -7358,7 +7364,7 @@
         <v>2301</v>
       </c>
       <c r="D119" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="E119" t="s">
         <v>152</v>
@@ -7381,7 +7387,7 @@
         <v>2302</v>
       </c>
       <c r="D120" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="E120" t="s">
         <v>154</v>
@@ -7404,7 +7410,7 @@
         <v>2303</v>
       </c>
       <c r="D121" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="E121" t="s">
         <v>155</v>
@@ -7427,7 +7433,7 @@
         <v>2401</v>
       </c>
       <c r="D122" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="E122" t="s">
         <v>684</v>
@@ -7450,7 +7456,7 @@
         <v>2503</v>
       </c>
       <c r="D123" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="E123" t="s">
         <v>156</v>
@@ -7473,7 +7479,7 @@
         <v>2504</v>
       </c>
       <c r="D124" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="E124" t="s">
         <v>158</v>
@@ -7496,7 +7502,7 @@
         <v>2601</v>
       </c>
       <c r="D125" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="E125" t="s">
         <v>160</v>
@@ -7519,7 +7525,7 @@
         <v>2701</v>
       </c>
       <c r="D126" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="E126" t="s">
         <v>162</v>
@@ -7542,7 +7548,7 @@
         <v>2702</v>
       </c>
       <c r="D127" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="E127" t="s">
         <v>164</v>
@@ -7565,7 +7571,7 @@
         <v>2802</v>
       </c>
       <c r="D128" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="E128" t="s">
         <v>166</v>
@@ -7588,7 +7594,7 @@
         <v>3002</v>
       </c>
       <c r="D129" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="E129" t="s">
         <v>167</v>
@@ -7611,7 +7617,7 @@
         <v>3201</v>
       </c>
       <c r="D130" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="E130" t="s">
         <v>168</v>
@@ -7634,7 +7640,7 @@
         <v>3301</v>
       </c>
       <c r="D131" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="E131" t="s">
         <v>170</v>
@@ -7657,7 +7663,7 @@
         <v>3601</v>
       </c>
       <c r="D132" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="E132" t="s">
         <v>172</v>
@@ -7680,7 +7686,7 @@
         <v>3602</v>
       </c>
       <c r="D133" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="E133" t="s">
         <v>174</v>
@@ -7703,7 +7709,7 @@
         <v>3603</v>
       </c>
       <c r="D134" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="E134" t="s">
         <v>176</v>
@@ -7726,7 +7732,7 @@
         <v>3604</v>
       </c>
       <c r="D135" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="E135" t="s">
         <v>178</v>
@@ -7749,7 +7755,7 @@
         <v>3701</v>
       </c>
       <c r="D136" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="E136" t="s">
         <v>685</v>
@@ -7772,7 +7778,7 @@
         <v>3702</v>
       </c>
       <c r="D137" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="E137" t="s">
         <v>179</v>
@@ -7795,7 +7801,7 @@
         <v>4001</v>
       </c>
       <c r="D138" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="E138" t="s">
         <v>181</v>
@@ -7818,7 +7824,7 @@
         <v>4101</v>
       </c>
       <c r="D139" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="E139" t="s">
         <v>686</v>
@@ -7841,7 +7847,7 @@
         <v>4201</v>
       </c>
       <c r="D140" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="E140" t="s">
         <v>183</v>
@@ -7864,7 +7870,7 @@
         <v>4301</v>
       </c>
       <c r="D141" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="E141" t="s">
         <v>687</v>
@@ -7887,7 +7893,7 @@
         <v>4302</v>
       </c>
       <c r="D142" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="E142" t="s">
         <v>689</v>
@@ -7910,7 +7916,7 @@
         <v>4401</v>
       </c>
       <c r="D143" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="E143" t="s">
         <v>185</v>
@@ -7933,7 +7939,7 @@
         <v>4801</v>
       </c>
       <c r="D144" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="E144" t="s">
         <v>690</v>
@@ -7956,7 +7962,7 @@
         <v>4802</v>
       </c>
       <c r="D145" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="E145" t="s">
         <v>692</v>
@@ -7979,7 +7985,7 @@
         <v>4803</v>
       </c>
       <c r="D146" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="E146" t="s">
         <v>187</v>
@@ -8002,7 +8008,7 @@
         <v>4804</v>
       </c>
       <c r="D147" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="E147" t="s">
         <v>693</v>
@@ -8025,7 +8031,7 @@
         <v>4805</v>
       </c>
       <c r="D148" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="E148" t="s">
         <v>189</v>
@@ -8048,7 +8054,7 @@
         <v>5001</v>
       </c>
       <c r="D149" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="E149" t="s">
         <v>190</v>
@@ -8071,7 +8077,7 @@
         <v>5101</v>
       </c>
       <c r="D150" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="E150" t="s">
         <v>694</v>
@@ -8094,7 +8100,7 @@
         <v>5302</v>
       </c>
       <c r="D151" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="E151" t="s">
         <v>696</v>
@@ -8117,7 +8123,7 @@
         <v>5305</v>
       </c>
       <c r="D152" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="E152" t="s">
         <v>192</v>
@@ -8140,7 +8146,7 @@
         <v>5401</v>
       </c>
       <c r="D153" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="E153" t="s">
         <v>194</v>
@@ -8163,7 +8169,7 @@
         <v>5501</v>
       </c>
       <c r="D154" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="E154" t="s">
         <v>698</v>
@@ -8186,7 +8192,7 @@
         <v>5601</v>
       </c>
       <c r="D155" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="E155" t="s">
         <v>196</v>
@@ -8209,7 +8215,7 @@
         <v>5701</v>
       </c>
       <c r="D156" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="E156" t="s">
         <v>198</v>
@@ -8232,7 +8238,7 @@
         <v>5801</v>
       </c>
       <c r="D157" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="E157" t="s">
         <v>200</v>
@@ -8255,7 +8261,7 @@
         <v>6202</v>
       </c>
       <c r="D158" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="E158" t="s">
         <v>201</v>
@@ -8278,7 +8284,7 @@
         <v>6203</v>
       </c>
       <c r="D159" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="E159" t="s">
         <v>203</v>
@@ -8301,7 +8307,7 @@
         <v>6301</v>
       </c>
       <c r="D160" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="E160" t="s">
         <v>205</v>
@@ -8324,7 +8330,7 @@
         <v>6302</v>
       </c>
       <c r="D161" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="E161" t="s">
         <v>207</v>
@@ -8347,7 +8353,7 @@
         <v>6303</v>
       </c>
       <c r="D162" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="E162" t="s">
         <v>209</v>
@@ -8370,7 +8376,7 @@
         <v>6601</v>
       </c>
       <c r="D163" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="E163" t="s">
         <v>210</v>
@@ -8393,7 +8399,7 @@
         <v>6801</v>
       </c>
       <c r="D164" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="E164" t="s">
         <v>212</v>
@@ -8416,7 +8422,7 @@
         <v>6901</v>
       </c>
       <c r="D165" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="E165" t="s">
         <v>215</v>
@@ -8439,7 +8445,7 @@
         <v>7001</v>
       </c>
       <c r="D166" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="E166" t="s">
         <v>217</v>
@@ -8462,7 +8468,7 @@
         <v>7401</v>
       </c>
       <c r="D167" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="E167" t="s">
         <v>219</v>
@@ -8485,7 +8491,7 @@
         <v>7402</v>
       </c>
       <c r="D168" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="E168" t="s">
         <v>221</v>
@@ -8508,7 +8514,7 @@
         <v>7403</v>
       </c>
       <c r="D169" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="E169" t="s">
         <v>700</v>
@@ -8531,7 +8537,7 @@
         <v>7601</v>
       </c>
       <c r="D170" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="E170" t="s">
         <v>222</v>
@@ -8554,7 +8560,7 @@
         <v>8401</v>
       </c>
       <c r="D171" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="E171" t="s">
         <v>224</v>
@@ -8577,7 +8583,7 @@
         <v>8402</v>
       </c>
       <c r="D172" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="E172" t="s">
         <v>226</v>
@@ -8600,7 +8606,7 @@
         <v>8403</v>
       </c>
       <c r="D173" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="E173" t="s">
         <v>227</v>
@@ -8623,7 +8629,7 @@
         <v>8501</v>
       </c>
       <c r="D174" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="E174" t="s">
         <v>228</v>
@@ -8646,7 +8652,7 @@
         <v>8901</v>
       </c>
       <c r="D175" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="E175" t="s">
         <v>230</v>
@@ -8669,7 +8675,7 @@
         <v>9001</v>
       </c>
       <c r="D176" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="E176" t="s">
         <v>232</v>
@@ -8692,7 +8698,7 @@
         <v>9101</v>
       </c>
       <c r="D177" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="E177" t="s">
         <v>234</v>
@@ -8715,7 +8721,7 @@
         <v>9102</v>
       </c>
       <c r="D178" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="E178" t="s">
         <v>235</v>
@@ -8738,7 +8744,7 @@
         <v>9201</v>
       </c>
       <c r="D179" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="E179" t="s">
         <v>236</v>
@@ -8761,7 +8767,7 @@
         <v>9301</v>
       </c>
       <c r="D180" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E180" t="s">
         <v>238</v>
@@ -8784,7 +8790,7 @@
         <v>9601</v>
       </c>
       <c r="D181" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="E181" t="s">
         <v>240</v>
@@ -8807,7 +8813,7 @@
         <v>9701</v>
       </c>
       <c r="D182" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="E182" t="s">
         <v>242</v>
@@ -8830,7 +8836,7 @@
         <v>9702</v>
       </c>
       <c r="D183" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="E183" t="s">
         <v>244</v>
@@ -8853,7 +8859,7 @@
         <v>10301</v>
       </c>
       <c r="D184" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="E184" t="s">
         <v>249</v>
@@ -8876,7 +8882,7 @@
         <v>10601</v>
       </c>
       <c r="D185" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="E185" t="s">
         <v>253</v>
@@ -8899,7 +8905,7 @@
         <v>10801</v>
       </c>
       <c r="D186" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="E186" t="s">
         <v>701</v>
@@ -8922,7 +8928,7 @@
         <v>10802</v>
       </c>
       <c r="D187" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="E187" t="s">
         <v>254</v>
@@ -8945,7 +8951,7 @@
         <v>10803</v>
       </c>
       <c r="D188" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="E188" t="s">
         <v>256</v>
@@ -8968,7 +8974,7 @@
         <v>10804</v>
       </c>
       <c r="D189" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="E189" t="s">
         <v>257</v>
@@ -8991,7 +8997,7 @@
         <v>11001</v>
       </c>
       <c r="D190" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="E190" t="s">
         <v>259</v>
@@ -9014,7 +9020,7 @@
         <v>11101</v>
       </c>
       <c r="D191" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="E191" t="s">
         <v>261</v>
@@ -9037,7 +9043,7 @@
         <v>11201</v>
       </c>
       <c r="D192" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="E192" t="s">
         <v>263</v>
@@ -9060,7 +9066,7 @@
         <v>11301</v>
       </c>
       <c r="D193" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="E193" t="s">
         <v>265</v>
@@ -9083,7 +9089,7 @@
         <v>11302</v>
       </c>
       <c r="D194" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="E194" t="s">
         <v>267</v>
@@ -9106,7 +9112,7 @@
         <v>11601</v>
       </c>
       <c r="D195" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="E195" t="s">
         <v>268</v>
@@ -9129,7 +9135,7 @@
         <v>11602</v>
       </c>
       <c r="D196" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="E196" t="s">
         <v>270</v>
@@ -9152,7 +9158,7 @@
         <v>11603</v>
       </c>
       <c r="D197" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="E197" t="s">
         <v>272</v>
@@ -9175,7 +9181,7 @@
         <v>11604</v>
       </c>
       <c r="D198" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="E198" t="s">
         <v>274</v>
@@ -9198,7 +9204,7 @@
         <v>11801</v>
       </c>
       <c r="D199" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="E199" t="s">
         <v>275</v>
@@ -9221,7 +9227,7 @@
         <v>11901</v>
       </c>
       <c r="D200" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="E200" t="s">
         <v>276</v>
@@ -9244,7 +9250,7 @@
         <v>12101</v>
       </c>
       <c r="D201" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="E201" t="s">
         <v>277</v>
@@ -9267,7 +9273,7 @@
         <v>12201</v>
       </c>
       <c r="D202" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="E202" t="s">
         <v>279</v>
@@ -9290,7 +9296,7 @@
         <v>12301</v>
       </c>
       <c r="D203" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="E203" t="s">
         <v>702</v>
@@ -9313,7 +9319,7 @@
         <v>12801</v>
       </c>
       <c r="D204" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="E204" t="s">
         <v>280</v>
@@ -9336,7 +9342,7 @@
         <v>12802</v>
       </c>
       <c r="D205" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="E205" t="s">
         <v>283</v>
@@ -9359,7 +9365,7 @@
         <v>12804</v>
       </c>
       <c r="D206" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="E206" t="s">
         <v>285</v>
@@ -9382,7 +9388,7 @@
         <v>12805</v>
       </c>
       <c r="D207" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="E207" t="s">
         <v>287</v>
@@ -9405,7 +9411,7 @@
         <v>12806</v>
       </c>
       <c r="D208" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="E208" t="s">
         <v>289</v>
@@ -9428,7 +9434,7 @@
         <v>13101</v>
       </c>
       <c r="D209" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="E209" t="s">
         <v>291</v>
@@ -9451,7 +9457,7 @@
         <v>13301</v>
       </c>
       <c r="D210" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="E210" t="s">
         <v>293</v>
@@ -9474,7 +9480,7 @@
         <v>13501</v>
       </c>
       <c r="D211" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="E211" t="s">
         <v>295</v>
@@ -9497,7 +9503,7 @@
         <v>13502</v>
       </c>
       <c r="D212" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="E212" t="s">
         <v>297</v>
@@ -9520,7 +9526,7 @@
         <v>13503</v>
       </c>
       <c r="D213" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="E213" t="s">
         <v>299</v>
@@ -9543,7 +9549,7 @@
         <v>13504</v>
       </c>
       <c r="D214" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
       <c r="E214" t="s">
         <v>704</v>
@@ -9566,7 +9572,7 @@
         <v>13701</v>
       </c>
       <c r="D215" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="E215" t="s">
         <v>301</v>
@@ -9589,7 +9595,7 @@
         <v>13702</v>
       </c>
       <c r="D216" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
       <c r="E216" t="s">
         <v>303</v>
@@ -9612,7 +9618,7 @@
         <v>13801</v>
       </c>
       <c r="D217" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="E217" t="s">
         <v>304</v>
@@ -9635,7 +9641,7 @@
         <v>13802</v>
       </c>
       <c r="D218" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="E218" t="s">
         <v>306</v>
@@ -9658,7 +9664,7 @@
         <v>13901</v>
       </c>
       <c r="D219" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="E219" t="s">
         <v>705</v>
@@ -9681,7 +9687,7 @@
         <v>14201</v>
       </c>
       <c r="D220" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="E220" t="s">
         <v>307</v>
@@ -9704,7 +9710,7 @@
         <v>14301</v>
       </c>
       <c r="D221" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="E221" t="s">
         <v>309</v>
@@ -9727,7 +9733,7 @@
         <v>14401</v>
       </c>
       <c r="D222" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="E222" t="s">
         <v>707</v>
@@ -9750,7 +9756,7 @@
         <v>14502</v>
       </c>
       <c r="D223" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="E223" t="s">
         <v>311</v>
@@ -9773,7 +9779,7 @@
         <v>14503</v>
       </c>
       <c r="D224" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="E224" t="s">
         <v>313</v>
@@ -9796,7 +9802,7 @@
         <v>14701</v>
       </c>
       <c r="D225" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="E225" t="s">
         <v>314</v>
@@ -9819,7 +9825,7 @@
         <v>14801</v>
       </c>
       <c r="D226" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="E226" t="s">
         <v>316</v>
@@ -9842,7 +9848,7 @@
         <v>14802</v>
       </c>
       <c r="D227" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="E227" t="s">
         <v>709</v>
@@ -9865,7 +9871,7 @@
         <v>15001</v>
       </c>
       <c r="D228" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="E228" t="s">
         <v>318</v>
@@ -9888,7 +9894,7 @@
         <v>15101</v>
       </c>
       <c r="D229" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="E229" t="s">
         <v>711</v>
@@ -9911,7 +9917,7 @@
         <v>15201</v>
       </c>
       <c r="D230" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="E230" t="s">
         <v>320</v>
@@ -9934,7 +9940,7 @@
         <v>15301</v>
       </c>
       <c r="D231" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="E231" t="s">
         <v>322</v>
@@ -9957,7 +9963,7 @@
         <v>15302</v>
       </c>
       <c r="D232" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="E232" t="s">
         <v>324</v>
@@ -9980,7 +9986,7 @@
         <v>15401</v>
       </c>
       <c r="D233" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="E233" t="s">
         <v>326</v>
@@ -10003,7 +10009,7 @@
         <v>15403</v>
       </c>
       <c r="D234" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="E234" t="s">
         <v>327</v>
@@ -10026,7 +10032,7 @@
         <v>15404</v>
       </c>
       <c r="D235" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="E235" t="s">
         <v>329</v>
@@ -10049,7 +10055,7 @@
         <v>15501</v>
       </c>
       <c r="D236" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="E236" t="s">
         <v>331</v>
@@ -10072,7 +10078,7 @@
         <v>15701</v>
       </c>
       <c r="D237" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="E237" t="s">
         <v>332</v>
@@ -10095,7 +10101,7 @@
         <v>16101</v>
       </c>
       <c r="D238" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="E238" t="s">
         <v>333</v>
@@ -10118,7 +10124,7 @@
         <v>16201</v>
       </c>
       <c r="D239" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="E239" t="s">
         <v>335</v>
@@ -10141,7 +10147,7 @@
         <v>16401</v>
       </c>
       <c r="D240" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="E240" t="s">
         <v>337</v>
@@ -10164,7 +10170,7 @@
         <v>16501</v>
       </c>
       <c r="D241" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="E241" t="s">
         <v>338</v>
@@ -10187,7 +10193,7 @@
         <v>16601</v>
       </c>
       <c r="D242" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="E242" t="s">
         <v>340</v>
@@ -10210,7 +10216,7 @@
         <v>16602</v>
       </c>
       <c r="D243" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="E243" t="s">
         <v>342</v>
@@ -10233,7 +10239,7 @@
         <v>16901</v>
       </c>
       <c r="D244" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="E244" t="s">
         <v>344</v>
@@ -10256,7 +10262,7 @@
         <v>17201</v>
       </c>
       <c r="D245" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="E245" t="s">
         <v>712</v>
@@ -10279,7 +10285,7 @@
         <v>17401</v>
       </c>
       <c r="D246" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="E246" t="s">
         <v>345</v>
@@ -10302,7 +10308,7 @@
         <v>17501</v>
       </c>
       <c r="D247" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="E247" t="s">
         <v>346</v>
@@ -10325,7 +10331,7 @@
         <v>17601</v>
       </c>
       <c r="D248" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="E248" t="s">
         <v>348</v>
@@ -10348,7 +10354,7 @@
         <v>17602</v>
       </c>
       <c r="D249" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="E249" t="s">
         <v>349</v>
@@ -10371,7 +10377,7 @@
         <v>17603</v>
       </c>
       <c r="D250" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="E250" t="s">
         <v>350</v>
@@ -10394,7 +10400,7 @@
         <v>17701</v>
       </c>
       <c r="D251" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="E251" t="s">
         <v>714</v>
@@ -10417,7 +10423,7 @@
         <v>17702</v>
       </c>
       <c r="D252" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="E252" t="s">
         <v>716</v>
@@ -10440,7 +10446,7 @@
         <v>17703</v>
       </c>
       <c r="D253" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="E253" t="s">
         <v>718</v>
@@ -10463,7 +10469,7 @@
         <v>17704</v>
       </c>
       <c r="D254" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="E254" t="s">
         <v>719</v>
@@ -10486,7 +10492,7 @@
         <v>17705</v>
       </c>
       <c r="D255" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="E255" t="s">
         <v>351</v>
@@ -10509,7 +10515,7 @@
         <v>17801</v>
       </c>
       <c r="D256" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="E256" t="s">
         <v>353</v>
@@ -10532,7 +10538,7 @@
         <v>18001</v>
       </c>
       <c r="D257" t="s">
-        <v>1084</v>
+        <v>1081</v>
       </c>
       <c r="E257" t="s">
         <v>355</v>
@@ -10555,7 +10561,7 @@
         <v>18101</v>
       </c>
       <c r="D258" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="E258" t="s">
         <v>357</v>
@@ -10578,7 +10584,7 @@
         <v>18501</v>
       </c>
       <c r="D259" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="E259" t="s">
         <v>358</v>
@@ -10601,7 +10607,7 @@
         <v>18601</v>
       </c>
       <c r="D260" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="E260" t="s">
         <v>720</v>
@@ -10624,7 +10630,7 @@
         <v>18801</v>
       </c>
       <c r="D261" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="E261" t="s">
         <v>360</v>
@@ -10647,7 +10653,7 @@
         <v>18901</v>
       </c>
       <c r="D262" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="E262" t="s">
         <v>362</v>
@@ -10670,7 +10676,7 @@
         <v>19101</v>
       </c>
       <c r="D263" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="E263" t="s">
         <v>721</v>
@@ -10693,7 +10699,7 @@
         <v>19201</v>
       </c>
       <c r="D264" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="E264" t="s">
         <v>363</v>
@@ -10716,7 +10722,7 @@
         <v>19301</v>
       </c>
       <c r="D265" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="E265" t="s">
         <v>723</v>
@@ -10739,7 +10745,7 @@
         <v>19501</v>
       </c>
       <c r="D266" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="E266" t="s">
         <v>364</v>
@@ -10762,7 +10768,7 @@
         <v>19601</v>
       </c>
       <c r="D267" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
       <c r="E267" t="s">
         <v>725</v>
@@ -10785,7 +10791,7 @@
         <v>20001</v>
       </c>
       <c r="D268" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="E268" t="s">
         <v>366</v>
@@ -10808,7 +10814,7 @@
         <v>20201</v>
       </c>
       <c r="D269" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
       <c r="E269" t="s">
         <v>367</v>
@@ -10831,7 +10837,7 @@
         <v>20202</v>
       </c>
       <c r="D270" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="E270" t="s">
         <v>368</v>
@@ -10854,7 +10860,7 @@
         <v>20301</v>
       </c>
       <c r="D271" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="E271" t="s">
         <v>730</v>
@@ -10877,7 +10883,7 @@
         <v>20401</v>
       </c>
       <c r="D272" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="E272" t="s">
         <v>369</v>
@@ -10900,7 +10906,7 @@
         <v>20702</v>
       </c>
       <c r="D273" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="E273" t="s">
         <v>371</v>
@@ -10923,7 +10929,7 @@
         <v>20801</v>
       </c>
       <c r="D274" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="E274" t="s">
         <v>372</v>
@@ -10946,7 +10952,7 @@
         <v>20901</v>
       </c>
       <c r="D275" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="E275" t="s">
         <v>731</v>
@@ -10969,7 +10975,7 @@
         <v>21001</v>
       </c>
       <c r="D276" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="E276" t="s">
         <v>733</v>
@@ -10992,7 +10998,7 @@
         <v>21101</v>
       </c>
       <c r="D277" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="E277" t="s">
         <v>373</v>
@@ -11015,7 +11021,7 @@
         <v>21501</v>
       </c>
       <c r="D278" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="E278" t="s">
         <v>375</v>
@@ -11038,7 +11044,7 @@
         <v>22001</v>
       </c>
       <c r="D279" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="E279" t="s">
         <v>377</v>
@@ -11061,7 +11067,7 @@
         <v>22201</v>
       </c>
       <c r="D280" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="E280" t="s">
         <v>378</v>
@@ -11084,7 +11090,7 @@
         <v>22401</v>
       </c>
       <c r="D281" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="E281" t="s">
         <v>380</v>
@@ -11107,7 +11113,7 @@
         <v>22402</v>
       </c>
       <c r="D282" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
       <c r="E282" t="s">
         <v>382</v>
@@ -11130,7 +11136,7 @@
         <v>22403</v>
       </c>
       <c r="D283" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="E283" t="s">
         <v>383</v>
@@ -11153,7 +11159,7 @@
         <v>22404</v>
       </c>
       <c r="D284" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="E284" t="s">
         <v>384</v>
@@ -11176,7 +11182,7 @@
         <v>22405</v>
       </c>
       <c r="D285" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="E285" t="s">
         <v>385</v>
@@ -11199,7 +11205,7 @@
         <v>22406</v>
       </c>
       <c r="D286" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
       <c r="E286" t="s">
         <v>386</v>
@@ -11222,7 +11228,7 @@
         <v>22601</v>
       </c>
       <c r="D287" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="E287" t="s">
         <v>388</v>
@@ -11245,7 +11251,7 @@
         <v>22701</v>
       </c>
       <c r="D288" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="E288" t="s">
         <v>735</v>
@@ -11268,7 +11274,7 @@
         <v>22702</v>
       </c>
       <c r="D289" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="E289" t="s">
         <v>390</v>
@@ -11291,7 +11297,7 @@
         <v>22703</v>
       </c>
       <c r="D290" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="E290" t="s">
         <v>737</v>
@@ -11314,7 +11320,7 @@
         <v>22901</v>
       </c>
       <c r="D291" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="E291" t="s">
         <v>392</v>
@@ -11337,7 +11343,7 @@
         <v>23001</v>
       </c>
       <c r="D292" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
       <c r="E292" t="s">
         <v>393</v>
@@ -11360,7 +11366,7 @@
         <v>23003</v>
       </c>
       <c r="D293" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="E293" t="s">
         <v>395</v>
@@ -11383,7 +11389,7 @@
         <v>23201</v>
       </c>
       <c r="D294" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="E294" t="s">
         <v>739</v>
@@ -11406,7 +11412,7 @@
         <v>23301</v>
       </c>
       <c r="D295" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="E295" t="s">
         <v>740</v>
@@ -11429,7 +11435,7 @@
         <v>23401</v>
       </c>
       <c r="D296" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="E296" t="s">
         <v>396</v>
@@ -11452,7 +11458,7 @@
         <v>23601</v>
       </c>
       <c r="D297" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="E297" t="s">
         <v>741</v>
@@ -11475,7 +11481,7 @@
         <v>23602</v>
       </c>
       <c r="D298" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="E298" t="s">
         <v>744</v>
@@ -11498,7 +11504,7 @@
         <v>23901</v>
       </c>
       <c r="D299" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="E299" t="s">
         <v>398</v>
@@ -11521,7 +11527,7 @@
         <v>23902</v>
       </c>
       <c r="D300" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="E300" t="s">
         <v>399</v>
@@ -11544,7 +11550,7 @@
         <v>24001</v>
       </c>
       <c r="D301" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="E301" t="s">
         <v>400</v>
@@ -11567,7 +11573,7 @@
         <v>24101</v>
       </c>
       <c r="D302" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="E302" t="s">
         <v>401</v>
@@ -11590,7 +11596,7 @@
         <v>24401</v>
       </c>
       <c r="D303" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
       <c r="E303" t="s">
         <v>746</v>
@@ -11613,7 +11619,7 @@
         <v>24402</v>
       </c>
       <c r="D304" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
       <c r="E304" t="s">
         <v>402</v>
@@ -11636,7 +11642,7 @@
         <v>24601</v>
       </c>
       <c r="D305" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
       <c r="E305" t="s">
         <v>403</v>
@@ -11659,7 +11665,7 @@
         <v>24701</v>
       </c>
       <c r="D306" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
       <c r="E306" t="s">
         <v>747</v>
@@ -11682,7 +11688,7 @@
         <v>24702</v>
       </c>
       <c r="D307" t="s">
-        <v>1134</v>
+        <v>1131</v>
       </c>
       <c r="E307" t="s">
         <v>749</v>
@@ -11705,7 +11711,7 @@
         <v>24801</v>
       </c>
       <c r="D308" t="s">
-        <v>1135</v>
+        <v>1132</v>
       </c>
       <c r="E308" t="s">
         <v>404</v>
@@ -11728,7 +11734,7 @@
         <v>24902</v>
       </c>
       <c r="D309" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
       <c r="E309" t="s">
         <v>750</v>
@@ -11751,7 +11757,7 @@
         <v>25102</v>
       </c>
       <c r="D310" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="E310" t="s">
         <v>406</v>
@@ -11774,7 +11780,7 @@
         <v>25103</v>
       </c>
       <c r="D311" t="s">
-        <v>1138</v>
+        <v>1135</v>
       </c>
       <c r="E311" t="s">
         <v>408</v>
@@ -11797,7 +11803,7 @@
         <v>25201</v>
       </c>
       <c r="D312" t="s">
-        <v>1139</v>
+        <v>1136</v>
       </c>
       <c r="E312" t="s">
         <v>410</v>
@@ -11820,7 +11826,7 @@
         <v>25301</v>
       </c>
       <c r="D313" t="s">
-        <v>1140</v>
+        <v>1137</v>
       </c>
       <c r="E313" t="s">
         <v>412</v>
@@ -11843,7 +11849,7 @@
         <v>25401</v>
       </c>
       <c r="D314" t="s">
-        <v>1141</v>
+        <v>1138</v>
       </c>
       <c r="E314" t="s">
         <v>413</v>
@@ -11866,7 +11872,7 @@
         <v>25601</v>
       </c>
       <c r="D315" t="s">
-        <v>1142</v>
+        <v>1139</v>
       </c>
       <c r="E315" t="s">
         <v>414</v>
@@ -11889,7 +11895,7 @@
         <v>25801</v>
       </c>
       <c r="D316" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
       <c r="E316" t="s">
         <v>416</v>
@@ -11912,7 +11918,7 @@
         <v>25901</v>
       </c>
       <c r="D317" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
       <c r="E317" t="s">
         <v>418</v>
@@ -11935,7 +11941,7 @@
         <v>26001</v>
       </c>
       <c r="D318" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
       <c r="E318" t="s">
         <v>420</v>
@@ -11958,7 +11964,7 @@
         <v>26002</v>
       </c>
       <c r="D319" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
       <c r="E319" t="s">
         <v>423</v>
@@ -11981,7 +11987,7 @@
         <v>26101</v>
       </c>
       <c r="D320" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="E320" t="s">
         <v>752</v>
@@ -12004,7 +12010,7 @@
         <v>26201</v>
       </c>
       <c r="D321" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="E321" t="s">
         <v>425</v>
@@ -12027,7 +12033,7 @@
         <v>26401</v>
       </c>
       <c r="D322" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="E322" t="s">
         <v>754</v>
@@ -12050,7 +12056,7 @@
         <v>26501</v>
       </c>
       <c r="D323" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
       <c r="E323" t="s">
         <v>426</v>
@@ -12073,7 +12079,7 @@
         <v>26601</v>
       </c>
       <c r="D324" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
       <c r="E324" t="s">
         <v>427</v>
@@ -12096,7 +12102,7 @@
         <v>26602</v>
       </c>
       <c r="D325" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
       <c r="E325" t="s">
         <v>428</v>
@@ -12119,7 +12125,7 @@
         <v>26603</v>
       </c>
       <c r="D326" t="s">
-        <v>1153</v>
+        <v>1150</v>
       </c>
       <c r="E326" t="s">
         <v>429</v>
@@ -12142,7 +12148,7 @@
         <v>26604</v>
       </c>
       <c r="D327" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="E327" t="s">
         <v>430</v>
@@ -12165,7 +12171,7 @@
         <v>26605</v>
       </c>
       <c r="D328" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="E328" t="s">
         <v>431</v>
@@ -12188,7 +12194,7 @@
         <v>26606</v>
       </c>
       <c r="D329" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="E329" t="s">
         <v>755</v>
@@ -12211,7 +12217,7 @@
         <v>26701</v>
       </c>
       <c r="D330" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="E330" t="s">
         <v>757</v>
@@ -12234,7 +12240,7 @@
         <v>26801</v>
       </c>
       <c r="D331" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="E331" t="s">
         <v>432</v>
@@ -12257,7 +12263,7 @@
         <v>26901</v>
       </c>
       <c r="D332" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="E332" t="s">
         <v>434</v>
@@ -12280,7 +12286,7 @@
         <v>27301</v>
       </c>
       <c r="D333" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="E333" t="s">
         <v>436</v>
@@ -12303,7 +12309,7 @@
         <v>27302</v>
       </c>
       <c r="D334" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="E334" t="s">
         <v>438</v>
@@ -12326,7 +12332,7 @@
         <v>27501</v>
       </c>
       <c r="D335" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
       <c r="E335" t="s">
         <v>440</v>
@@ -12349,7 +12355,7 @@
         <v>27601</v>
       </c>
       <c r="D336" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="E336" t="s">
         <v>442</v>
@@ -12372,7 +12378,7 @@
         <v>27701</v>
       </c>
       <c r="D337" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="E337" t="s">
         <v>443</v>
@@ -12395,7 +12401,7 @@
         <v>28001</v>
       </c>
       <c r="D338" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="E338" t="s">
         <v>444</v>
@@ -12418,7 +12424,7 @@
         <v>28002</v>
       </c>
       <c r="D339" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="E339" t="s">
         <v>446</v>
@@ -12441,7 +12447,7 @@
         <v>28003</v>
       </c>
       <c r="D340" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
       <c r="E340" t="s">
         <v>448</v>
@@ -12464,7 +12470,7 @@
         <v>28101</v>
       </c>
       <c r="D341" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="E341" t="s">
         <v>449</v>
@@ -12487,7 +12493,7 @@
         <v>28102</v>
       </c>
       <c r="D342" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="E342" t="s">
         <v>451</v>
@@ -12510,7 +12516,7 @@
         <v>28103</v>
       </c>
       <c r="D343" t="s">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="E343" t="s">
         <v>453</v>
@@ -12533,7 +12539,7 @@
         <v>28104</v>
       </c>
       <c r="D344" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="E344" t="s">
         <v>454</v>
@@ -12556,7 +12562,7 @@
         <v>28105</v>
       </c>
       <c r="D345" t="s">
-        <v>1172</v>
+        <v>1169</v>
       </c>
       <c r="E345" t="s">
         <v>455</v>
@@ -12579,7 +12585,7 @@
         <v>28401</v>
       </c>
       <c r="D346" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
       <c r="E346" t="s">
         <v>456</v>
@@ -12602,7 +12608,7 @@
         <v>28501</v>
       </c>
       <c r="D347" t="s">
-        <v>1174</v>
+        <v>1171</v>
       </c>
       <c r="E347" t="s">
         <v>458</v>
@@ -12625,7 +12631,7 @@
         <v>28503</v>
       </c>
       <c r="D348" t="s">
-        <v>1175</v>
+        <v>1172</v>
       </c>
       <c r="E348" t="s">
         <v>459</v>
@@ -12648,7 +12654,7 @@
         <v>28601</v>
       </c>
       <c r="D349" t="s">
-        <v>1176</v>
+        <v>1173</v>
       </c>
       <c r="E349" t="s">
         <v>759</v>
@@ -12671,7 +12677,7 @@
         <v>28701</v>
       </c>
       <c r="D350" t="s">
-        <v>1177</v>
+        <v>1174</v>
       </c>
       <c r="E350" t="s">
         <v>761</v>
@@ -12694,7 +12700,7 @@
         <v>28801</v>
       </c>
       <c r="D351" t="s">
-        <v>1178</v>
+        <v>1175</v>
       </c>
       <c r="E351" t="s">
         <v>460</v>
@@ -12717,7 +12723,7 @@
         <v>28901</v>
       </c>
       <c r="D352" t="s">
-        <v>1179</v>
+        <v>1176</v>
       </c>
       <c r="E352" t="s">
         <v>462</v>
@@ -12740,7 +12746,7 @@
         <v>29001</v>
       </c>
       <c r="D353" t="s">
-        <v>1180</v>
+        <v>1177</v>
       </c>
       <c r="E353" t="s">
         <v>463</v>
@@ -12763,7 +12769,7 @@
         <v>29101</v>
       </c>
       <c r="D354" t="s">
-        <v>1181</v>
+        <v>1178</v>
       </c>
       <c r="E354" t="s">
         <v>464</v>
@@ -12786,7 +12792,7 @@
         <v>29102</v>
       </c>
       <c r="D355" t="s">
-        <v>1182</v>
+        <v>1179</v>
       </c>
       <c r="E355" t="s">
         <v>466</v>
@@ -12809,7 +12815,7 @@
         <v>29201</v>
       </c>
       <c r="D356" t="s">
-        <v>1183</v>
+        <v>1180</v>
       </c>
       <c r="E356" t="s">
         <v>468</v>
@@ -12832,7 +12838,7 @@
         <v>29401</v>
       </c>
       <c r="D357" t="s">
-        <v>1184</v>
+        <v>1181</v>
       </c>
       <c r="E357" t="s">
         <v>469</v>
@@ -12855,7 +12861,7 @@
         <v>29501</v>
       </c>
       <c r="D358" t="s">
-        <v>1185</v>
+        <v>1182</v>
       </c>
       <c r="E358" t="s">
         <v>471</v>
@@ -12878,7 +12884,7 @@
         <v>29601</v>
       </c>
       <c r="D359" t="s">
-        <v>1186</v>
+        <v>1183</v>
       </c>
       <c r="E359" t="s">
         <v>473</v>
@@ -12901,7 +12907,7 @@
         <v>30201</v>
       </c>
       <c r="D360" t="s">
-        <v>1187</v>
+        <v>1184</v>
       </c>
       <c r="E360" t="s">
         <v>475</v>
@@ -12924,7 +12930,7 @@
         <v>30301</v>
       </c>
       <c r="D361" t="s">
-        <v>1188</v>
+        <v>1185</v>
       </c>
       <c r="E361" t="s">
         <v>477</v>
@@ -12947,7 +12953,7 @@
         <v>30401</v>
       </c>
       <c r="D362" t="s">
-        <v>1189</v>
+        <v>1186</v>
       </c>
       <c r="E362" t="s">
         <v>479</v>
@@ -12970,7 +12976,7 @@
         <v>30402</v>
       </c>
       <c r="D363" t="s">
-        <v>1190</v>
+        <v>1187</v>
       </c>
       <c r="E363" t="s">
         <v>481</v>
@@ -12993,7 +12999,7 @@
         <v>30701</v>
       </c>
       <c r="D364" t="s">
-        <v>1191</v>
+        <v>1188</v>
       </c>
       <c r="E364" t="s">
         <v>483</v>
@@ -13016,7 +13022,7 @@
         <v>30801</v>
       </c>
       <c r="D365" t="s">
-        <v>1192</v>
+        <v>1189</v>
       </c>
       <c r="E365" t="s">
         <v>763</v>
@@ -13039,7 +13045,7 @@
         <v>30901</v>
       </c>
       <c r="D366" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
       <c r="E366" t="s">
         <v>484</v>
@@ -13062,7 +13068,7 @@
         <v>31201</v>
       </c>
       <c r="D367" t="s">
-        <v>1194</v>
+        <v>1191</v>
       </c>
       <c r="E367" t="s">
         <v>486</v>
@@ -13085,7 +13091,7 @@
         <v>31302</v>
       </c>
       <c r="D368" t="s">
-        <v>1195</v>
+        <v>1192</v>
       </c>
       <c r="E368" t="s">
         <v>487</v>
@@ -13108,7 +13114,7 @@
         <v>31304</v>
       </c>
       <c r="D369" t="s">
-        <v>1196</v>
+        <v>1193</v>
       </c>
       <c r="E369" t="s">
         <v>764</v>
@@ -13131,7 +13137,7 @@
         <v>31501</v>
       </c>
       <c r="D370" t="s">
-        <v>1197</v>
+        <v>1194</v>
       </c>
       <c r="E370" t="s">
         <v>489</v>
@@ -13154,7 +13160,7 @@
         <v>31901</v>
       </c>
       <c r="D371" t="s">
-        <v>1198</v>
+        <v>1195</v>
       </c>
       <c r="E371" t="s">
         <v>490</v>
@@ -13177,7 +13183,7 @@
         <v>32001</v>
       </c>
       <c r="D372" t="s">
-        <v>1199</v>
+        <v>1196</v>
       </c>
       <c r="E372" t="s">
         <v>491</v>
@@ -13200,7 +13206,7 @@
         <v>32201</v>
       </c>
       <c r="D373" t="s">
-        <v>1200</v>
+        <v>1197</v>
       </c>
       <c r="E373" t="s">
         <v>766</v>
@@ -13223,7 +13229,7 @@
         <v>32401</v>
       </c>
       <c r="D374" t="s">
-        <v>1201</v>
+        <v>1198</v>
       </c>
       <c r="E374" t="s">
         <v>493</v>
@@ -13246,7 +13252,7 @@
         <v>32501</v>
       </c>
       <c r="D375" t="s">
-        <v>1202</v>
+        <v>1199</v>
       </c>
       <c r="E375" t="s">
         <v>495</v>
@@ -13269,7 +13275,7 @@
         <v>32701</v>
       </c>
       <c r="D376" t="s">
-        <v>1203</v>
+        <v>1200</v>
       </c>
       <c r="E376" t="s">
         <v>496</v>
@@ -13292,7 +13298,7 @@
         <v>33001</v>
       </c>
       <c r="D377" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
       <c r="E377" t="s">
         <v>498</v>
@@ -13315,7 +13321,7 @@
         <v>33101</v>
       </c>
       <c r="D378" t="s">
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="E378" t="s">
         <v>500</v>
@@ -13338,7 +13344,7 @@
         <v>33401</v>
       </c>
       <c r="D379" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
       <c r="E379" t="s">
         <v>501</v>
@@ -13361,7 +13367,7 @@
         <v>33701</v>
       </c>
       <c r="D380" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="E380" t="s">
         <v>503</v>
@@ -13384,7 +13390,7 @@
         <v>33702</v>
       </c>
       <c r="D381" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="E381" t="s">
         <v>504</v>
@@ -13407,7 +13413,7 @@
         <v>33801</v>
       </c>
       <c r="D382" t="s">
-        <v>1209</v>
+        <v>1206</v>
       </c>
       <c r="E382" t="s">
         <v>505</v>
@@ -13430,7 +13436,7 @@
         <v>33901</v>
       </c>
       <c r="D383" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="E383" t="s">
         <v>768</v>
@@ -13453,7 +13459,7 @@
         <v>34001</v>
       </c>
       <c r="D384" t="s">
-        <v>1211</v>
+        <v>1208</v>
       </c>
       <c r="E384" t="s">
         <v>507</v>
@@ -13476,7 +13482,7 @@
         <v>34101</v>
       </c>
       <c r="D385" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="E385" t="s">
         <v>509</v>
@@ -13499,7 +13505,7 @@
         <v>34201</v>
       </c>
       <c r="D386" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="E386" t="s">
         <v>770</v>
@@ -13522,7 +13528,7 @@
         <v>34301</v>
       </c>
       <c r="D387" t="s">
-        <v>1214</v>
+        <v>1211</v>
       </c>
       <c r="E387" t="s">
         <v>510</v>
@@ -13545,7 +13551,7 @@
         <v>34501</v>
       </c>
       <c r="D388" t="s">
-        <v>1215</v>
+        <v>1212</v>
       </c>
       <c r="E388" t="s">
         <v>512</v>
@@ -13568,7 +13574,7 @@
         <v>34601</v>
       </c>
       <c r="D389" t="s">
-        <v>1216</v>
+        <v>1213</v>
       </c>
       <c r="E389" t="s">
         <v>514</v>
@@ -13591,7 +13597,7 @@
         <v>34801</v>
       </c>
       <c r="D390" t="s">
-        <v>1217</v>
+        <v>1214</v>
       </c>
       <c r="E390" t="s">
         <v>771</v>
@@ -13614,7 +13620,7 @@
         <v>35001</v>
       </c>
       <c r="D391" t="s">
-        <v>1218</v>
+        <v>1215</v>
       </c>
       <c r="E391" t="s">
         <v>517</v>
@@ -13637,7 +13643,7 @@
         <v>35101</v>
       </c>
       <c r="D392" t="s">
-        <v>1219</v>
+        <v>1216</v>
       </c>
       <c r="E392" t="s">
         <v>518</v>
@@ -13660,7 +13666,7 @@
         <v>35301</v>
       </c>
       <c r="D393" t="s">
-        <v>1220</v>
+        <v>1217</v>
       </c>
       <c r="E393" t="s">
         <v>519</v>
@@ -13683,7 +13689,7 @@
         <v>35402</v>
       </c>
       <c r="D394" t="s">
-        <v>1221</v>
+        <v>1218</v>
       </c>
       <c r="E394" t="s">
         <v>521</v>
@@ -13706,7 +13712,7 @@
         <v>35602</v>
       </c>
       <c r="D395" t="s">
-        <v>1222</v>
+        <v>1219</v>
       </c>
       <c r="E395" t="s">
         <v>773</v>
@@ -13729,7 +13735,7 @@
         <v>35801</v>
       </c>
       <c r="D396" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="E396" t="s">
         <v>523</v>
@@ -13752,7 +13758,7 @@
         <v>35901</v>
       </c>
       <c r="D397" t="s">
-        <v>1224</v>
+        <v>1221</v>
       </c>
       <c r="E397" t="s">
         <v>525</v>
@@ -13775,7 +13781,7 @@
         <v>36001</v>
       </c>
       <c r="D398" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="E398" t="s">
         <v>775</v>
@@ -13798,7 +13804,7 @@
         <v>36101</v>
       </c>
       <c r="D399" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="E399" t="s">
         <v>526</v>
@@ -13821,7 +13827,7 @@
         <v>36201</v>
       </c>
       <c r="D400" t="s">
-        <v>1227</v>
+        <v>1224</v>
       </c>
       <c r="E400" t="s">
         <v>528</v>
@@ -13844,7 +13850,7 @@
         <v>36301</v>
       </c>
       <c r="D401" t="s">
-        <v>1228</v>
+        <v>1225</v>
       </c>
       <c r="E401" t="s">
         <v>529</v>
@@ -13867,7 +13873,7 @@
         <v>36401</v>
       </c>
       <c r="D402" t="s">
-        <v>1229</v>
+        <v>1226</v>
       </c>
       <c r="E402" t="s">
         <v>531</v>
@@ -13890,7 +13896,7 @@
         <v>36501</v>
       </c>
       <c r="D403" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
       <c r="E403" t="s">
         <v>533</v>
@@ -13913,7 +13919,7 @@
         <v>36701</v>
       </c>
       <c r="D404" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
       <c r="E404" t="s">
         <v>535</v>
@@ -13936,7 +13942,7 @@
         <v>36801</v>
       </c>
       <c r="D405" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="E405" t="s">
         <v>537</v>
@@ -13959,7 +13965,7 @@
         <v>36901</v>
       </c>
       <c r="D406" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="E406" t="s">
         <v>538</v>
@@ -13982,7 +13988,7 @@
         <v>37001</v>
       </c>
       <c r="D407" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
       <c r="E407" t="s">
         <v>540</v>
@@ -14005,7 +14011,7 @@
         <v>37101</v>
       </c>
       <c r="D408" t="s">
-        <v>1235</v>
+        <v>1232</v>
       </c>
       <c r="E408" t="s">
         <v>777</v>
@@ -14028,7 +14034,7 @@
         <v>37301</v>
       </c>
       <c r="D409" t="s">
-        <v>1236</v>
+        <v>1233</v>
       </c>
       <c r="E409" t="s">
         <v>542</v>
@@ -14051,7 +14057,7 @@
         <v>37501</v>
       </c>
       <c r="D410" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
       <c r="E410" t="s">
         <v>543</v>
@@ -14074,7 +14080,7 @@
         <v>37601</v>
       </c>
       <c r="D411" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="E411" t="s">
         <v>546</v>
@@ -14097,7 +14103,7 @@
         <v>37801</v>
       </c>
       <c r="D412" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
       <c r="E412" t="s">
         <v>547</v>
@@ -14120,7 +14126,7 @@
         <v>37802</v>
       </c>
       <c r="D413" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="E413" t="s">
         <v>549</v>
@@ -14143,7 +14149,7 @@
         <v>37803</v>
       </c>
       <c r="D414" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="E414" t="s">
         <v>550</v>
@@ -14166,7 +14172,7 @@
         <v>37804</v>
       </c>
       <c r="D415" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
       <c r="E415" t="s">
         <v>551</v>
@@ -14189,7 +14195,7 @@
         <v>37805</v>
       </c>
       <c r="D416" t="s">
-        <v>1243</v>
+        <v>1240</v>
       </c>
       <c r="E416" t="s">
         <v>552</v>
@@ -14212,7 +14218,7 @@
         <v>37806</v>
       </c>
       <c r="D417" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="E417" t="s">
         <v>553</v>
@@ -14235,7 +14241,7 @@
         <v>37807</v>
       </c>
       <c r="D418" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="E418" t="s">
         <v>555</v>
@@ -14258,7 +14264,7 @@
         <v>37901</v>
       </c>
       <c r="D419" t="s">
-        <v>1246</v>
+        <v>1243</v>
       </c>
       <c r="E419" t="s">
         <v>557</v>
@@ -14281,7 +14287,7 @@
         <v>38001</v>
       </c>
       <c r="D420" t="s">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="E420" t="s">
         <v>779</v>
@@ -14304,7 +14310,7 @@
         <v>38101</v>
       </c>
       <c r="D421" t="s">
-        <v>1248</v>
+        <v>1245</v>
       </c>
       <c r="E421" t="s">
         <v>559</v>
@@ -14327,7 +14333,7 @@
         <v>38301</v>
       </c>
       <c r="D422" t="s">
-        <v>1249</v>
+        <v>1246</v>
       </c>
       <c r="E422" t="s">
         <v>561</v>
@@ -14350,7 +14356,7 @@
         <v>38501</v>
       </c>
       <c r="D423" t="s">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="E423" t="s">
         <v>562</v>
@@ -14373,7 +14379,7 @@
         <v>38601</v>
       </c>
       <c r="D424" t="s">
-        <v>1251</v>
+        <v>1248</v>
       </c>
       <c r="E424" t="s">
         <v>564</v>
@@ -14396,7 +14402,7 @@
         <v>38701</v>
       </c>
       <c r="D425" t="s">
-        <v>1252</v>
+        <v>1249</v>
       </c>
       <c r="E425" t="s">
         <v>781</v>
@@ -14419,7 +14425,7 @@
         <v>38801</v>
       </c>
       <c r="D426" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="E426" t="s">
         <v>566</v>
@@ -14442,7 +14448,7 @@
         <v>38802</v>
       </c>
       <c r="D427" t="s">
-        <v>1254</v>
+        <v>1251</v>
       </c>
       <c r="E427" t="s">
         <v>568</v>
@@ -14465,7 +14471,7 @@
         <v>38803</v>
       </c>
       <c r="D428" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
       <c r="E428" t="s">
         <v>783</v>
@@ -14488,7 +14494,7 @@
         <v>38804</v>
       </c>
       <c r="D429" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
       <c r="E429" t="s">
         <v>570</v>
@@ -14511,7 +14517,7 @@
         <v>38805</v>
       </c>
       <c r="D430" t="s">
-        <v>1257</v>
+        <v>1254</v>
       </c>
       <c r="E430" t="s">
         <v>572</v>
@@ -14534,7 +14540,7 @@
         <v>38901</v>
       </c>
       <c r="D431" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="E431" t="s">
         <v>573</v>
@@ -15750,11 +15756,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G491">
-    <sortState ref="A2:O491">
-      <sortCondition ref="D1:D491"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>